<commit_message>
added search name to functions
</commit_message>
<xml_diff>
--- a/DTCalumni.xlsx
+++ b/DTCalumni.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/lina4225_ox_ac_uk/Documents/DTC Anniversary Conference/DTC21_scraper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89EA2037-EF52-D947-B129-B532B66798D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{89EA2037-EF52-D947-B129-B532B66798D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41E44EF9-6DE1-5647-BB98-A48B4AD4D50A}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15900" xr2:uid="{8E96BCEF-6501-0345-83A1-327230941FB1}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="36000" windowHeight="22520" xr2:uid="{8E96BCEF-6501-0345-83A1-327230941FB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -5849,10 +5852,13 @@
   <dimension ref="A1:S1110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="35.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>